<commit_message>
Refactor cargar_datos: mapeo directo de columnas Excel, simplificado y robusto
</commit_message>
<xml_diff>
--- a/Datos_Termicos.xlsx
+++ b/Datos_Termicos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://itcelaya.sharepoint.com/sites/MCI1Semestre/Documentos compartidos/DahboardMaestria/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{028FDFE4-5AE3-4FE7-8CAF-D06F626BFCE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="14" documentId="8_{028FDFE4-5AE3-4FE7-8CAF-D06F626BFCE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{64B3C0C9-0278-46ED-9265-08342EF1D541}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{F61F8C48-0298-494E-9746-CDE449CEB114}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="28800" windowHeight="15345" xr2:uid="{F61F8C48-0298-494E-9746-CDE449CEB114}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -668,8 +668,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{228467D4-AF78-4C51-B1ED-F10469F9D0CC}">
   <dimension ref="A1:W28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="T21" sqref="T21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -825,6 +825,12 @@
       <c r="S2" t="s">
         <v>29</v>
       </c>
+      <c r="T2">
+        <v>20</v>
+      </c>
+      <c r="U2">
+        <v>20</v>
+      </c>
       <c r="W2" t="s">
         <v>30</v>
       </c>
@@ -884,6 +890,12 @@
       <c r="S3" t="s">
         <v>35</v>
       </c>
+      <c r="T3">
+        <v>10</v>
+      </c>
+      <c r="U3">
+        <v>21</v>
+      </c>
       <c r="W3" t="s">
         <v>36</v>
       </c>
@@ -943,6 +955,12 @@
       <c r="S4" t="s">
         <v>29</v>
       </c>
+      <c r="T4">
+        <v>30</v>
+      </c>
+      <c r="U4">
+        <v>22</v>
+      </c>
       <c r="W4" t="s">
         <v>38</v>
       </c>
@@ -1002,6 +1020,12 @@
       <c r="S5" t="s">
         <v>29</v>
       </c>
+      <c r="T5">
+        <v>25</v>
+      </c>
+      <c r="U5">
+        <v>23</v>
+      </c>
       <c r="W5" t="s">
         <v>41</v>
       </c>
@@ -1061,6 +1085,12 @@
       <c r="S6" t="s">
         <v>29</v>
       </c>
+      <c r="T6">
+        <v>16</v>
+      </c>
+      <c r="U6">
+        <v>24</v>
+      </c>
       <c r="W6" t="s">
         <v>44</v>
       </c>
@@ -1120,6 +1150,12 @@
       <c r="S7" t="s">
         <v>45</v>
       </c>
+      <c r="T7">
+        <v>17</v>
+      </c>
+      <c r="U7">
+        <v>25</v>
+      </c>
       <c r="W7" t="s">
         <v>46</v>
       </c>
@@ -1179,6 +1215,12 @@
       <c r="S8" t="s">
         <v>49</v>
       </c>
+      <c r="T8">
+        <v>18</v>
+      </c>
+      <c r="U8">
+        <v>26</v>
+      </c>
       <c r="W8" t="s">
         <v>50</v>
       </c>
@@ -1238,6 +1280,12 @@
       <c r="S9" t="s">
         <v>35</v>
       </c>
+      <c r="T9">
+        <v>19</v>
+      </c>
+      <c r="U9">
+        <v>27</v>
+      </c>
       <c r="W9" t="s">
         <v>52</v>
       </c>
@@ -1297,6 +1345,12 @@
       <c r="S10" t="s">
         <v>29</v>
       </c>
+      <c r="T10">
+        <v>20</v>
+      </c>
+      <c r="U10">
+        <v>28</v>
+      </c>
       <c r="W10" t="s">
         <v>54</v>
       </c>
@@ -1356,6 +1410,12 @@
       <c r="S11" t="s">
         <v>29</v>
       </c>
+      <c r="T11">
+        <v>21</v>
+      </c>
+      <c r="U11">
+        <v>29</v>
+      </c>
       <c r="W11" t="s">
         <v>56</v>
       </c>
@@ -1415,6 +1475,12 @@
       <c r="S12" t="s">
         <v>35</v>
       </c>
+      <c r="T12">
+        <v>22</v>
+      </c>
+      <c r="U12">
+        <v>30</v>
+      </c>
       <c r="W12" t="s">
         <v>58</v>
       </c>
@@ -1474,6 +1540,12 @@
       <c r="S13" t="s">
         <v>29</v>
       </c>
+      <c r="T13">
+        <v>23</v>
+      </c>
+      <c r="U13">
+        <v>31</v>
+      </c>
       <c r="W13" t="s">
         <v>60</v>
       </c>
@@ -1533,6 +1605,12 @@
       <c r="S14" t="s">
         <v>35</v>
       </c>
+      <c r="T14">
+        <v>24</v>
+      </c>
+      <c r="U14">
+        <v>32</v>
+      </c>
       <c r="W14" t="s">
         <v>61</v>
       </c>
@@ -1592,6 +1670,12 @@
       <c r="S15" t="s">
         <v>35</v>
       </c>
+      <c r="T15">
+        <v>25</v>
+      </c>
+      <c r="U15">
+        <v>33</v>
+      </c>
       <c r="W15" t="s">
         <v>63</v>
       </c>
@@ -1651,6 +1735,12 @@
       <c r="S16" t="s">
         <v>35</v>
       </c>
+      <c r="T16">
+        <v>26</v>
+      </c>
+      <c r="U16">
+        <v>34</v>
+      </c>
       <c r="W16" t="s">
         <v>65</v>
       </c>
@@ -1710,6 +1800,12 @@
       <c r="S17" t="s">
         <v>49</v>
       </c>
+      <c r="T17">
+        <v>27</v>
+      </c>
+      <c r="U17">
+        <v>35</v>
+      </c>
       <c r="W17" t="s">
         <v>66</v>
       </c>
@@ -1769,6 +1865,12 @@
       <c r="S18" t="s">
         <v>29</v>
       </c>
+      <c r="T18">
+        <v>28</v>
+      </c>
+      <c r="U18">
+        <v>36</v>
+      </c>
       <c r="W18" t="s">
         <v>68</v>
       </c>
@@ -1828,6 +1930,12 @@
       <c r="S19" t="s">
         <v>29</v>
       </c>
+      <c r="T19">
+        <v>29</v>
+      </c>
+      <c r="U19">
+        <v>37</v>
+      </c>
       <c r="W19" t="s">
         <v>70</v>
       </c>
@@ -1887,6 +1995,12 @@
       <c r="S20" t="s">
         <v>35</v>
       </c>
+      <c r="T20">
+        <v>30</v>
+      </c>
+      <c r="U20">
+        <v>38</v>
+      </c>
       <c r="W20" t="s">
         <v>72</v>
       </c>
@@ -1946,6 +2060,12 @@
       <c r="S21" t="s">
         <v>45</v>
       </c>
+      <c r="T21">
+        <v>31</v>
+      </c>
+      <c r="U21">
+        <v>39</v>
+      </c>
       <c r="W21" t="s">
         <v>74</v>
       </c>
@@ -2005,6 +2125,12 @@
       <c r="S22" t="s">
         <v>49</v>
       </c>
+      <c r="T22">
+        <v>32</v>
+      </c>
+      <c r="U22">
+        <v>40</v>
+      </c>
       <c r="W22" t="s">
         <v>76</v>
       </c>
@@ -2064,6 +2190,12 @@
       <c r="S23" t="s">
         <v>35</v>
       </c>
+      <c r="T23">
+        <v>33</v>
+      </c>
+      <c r="U23">
+        <v>41</v>
+      </c>
       <c r="W23" t="s">
         <v>77</v>
       </c>
@@ -2123,6 +2255,12 @@
       <c r="S24" t="s">
         <v>49</v>
       </c>
+      <c r="T24">
+        <v>34</v>
+      </c>
+      <c r="U24">
+        <v>42</v>
+      </c>
       <c r="W24" t="s">
         <v>79</v>
       </c>
@@ -2182,6 +2320,12 @@
       <c r="S25" t="s">
         <v>49</v>
       </c>
+      <c r="T25">
+        <v>35</v>
+      </c>
+      <c r="U25">
+        <v>43</v>
+      </c>
       <c r="W25" t="s">
         <v>81</v>
       </c>
@@ -2241,6 +2385,12 @@
       <c r="S26" t="s">
         <v>35</v>
       </c>
+      <c r="T26">
+        <v>36</v>
+      </c>
+      <c r="U26">
+        <v>44</v>
+      </c>
       <c r="W26" t="s">
         <v>82</v>
       </c>
@@ -2300,6 +2450,12 @@
       <c r="S27" t="s">
         <v>49</v>
       </c>
+      <c r="T27">
+        <v>37</v>
+      </c>
+      <c r="U27">
+        <v>45</v>
+      </c>
       <c r="W27" t="s">
         <v>84</v>
       </c>
@@ -2359,6 +2515,12 @@
       <c r="S28" t="s">
         <v>49</v>
       </c>
+      <c r="T28">
+        <v>38</v>
+      </c>
+      <c r="U28">
+        <v>46</v>
+      </c>
       <c r="W28" t="s">
         <v>85</v>
       </c>
@@ -2366,4 +2528,257 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100ED905B610D6FEF4595837C95F07EE10F" ma:contentTypeVersion="11" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="54c9ca00a59293971885796178ed8f14">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="d635fad1-26cb-42e0-9992-67a0d96ad443" xmlns:ns3="6d1e0c5a-b588-4b3f-8915-8daad152d597" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3e5abccb938aec1be4a0371102652431" ns2:_="" ns3:_="">
+    <xsd:import namespace="d635fad1-26cb-42e0-9992-67a0d96ad443"/>
+    <xsd:import namespace="6d1e0c5a-b588-4b3f-8915-8daad152d597"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceSearchProperties" minOccurs="0"/>
+                <xsd:element ref="ns2:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
+                <xsd:element ref="ns3:TaxCatchAll" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaLengthInSeconds" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="d635fad1-26cb-42e0-9992-67a0d96ad443" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceSearchProperties" ma:index="10" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="12" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Etiquetas de imagen" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="0e3a4998-2801-4cba-859a-8a7848551807" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="14" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="15" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="16" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="17" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaLengthInSeconds" ma:index="18" nillable="true" ma:displayName="MediaLengthInSeconds" ma:hidden="true" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="6d1e0c5a-b588-4b3f-8915-8daad152d597" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="TaxCatchAll" ma:index="13" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{ec6c44ba-75a2-4275-bcbe-4ad39d13407b}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="6d1e0c5a-b588-4b3f-8915-8daad152d597">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Tipo de contenido"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Título"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="6d1e0c5a-b588-4b3f-8915-8daad152d597" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="d635fad1-26cb-42e0-9992-67a0d96ad443">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0C937263-9E08-4A0F-B29F-DD447503B35A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="d635fad1-26cb-42e0-9992-67a0d96ad443"/>
+    <ds:schemaRef ds:uri="6d1e0c5a-b588-4b3f-8915-8daad152d597"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A2BCFF91-0746-470F-BF44-B12583560FCA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="6d1e0c5a-b588-4b3f-8915-8daad152d597"/>
+    <ds:schemaRef ds:uri="d635fad1-26cb-42e0-9992-67a0d96ad443"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{741FF2F6-DAEB-42B8-94E9-8AC80B028C2E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>